<commit_message>
Better Style and Conversions
</commit_message>
<xml_diff>
--- a/Binary-ToandFromConvertor.xlsx
+++ b/Binary-ToandFromConvertor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sly\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE55432D-2B39-44DD-993D-DC88E023C4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAFB7A5-29EE-46DB-955C-617331678C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{D25947CC-B487-4CB0-9709-D77A5E30A7E4}"/>
+    <workbookView xWindow="20370" yWindow="-4665" windowWidth="29040" windowHeight="15720" xr2:uid="{D25947CC-B487-4CB0-9709-D77A5E30A7E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Conversions" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>Octal</t>
   </si>
@@ -46,15 +46,6 @@
     <t>Decimal</t>
   </si>
   <si>
-    <t>C8A5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Hex to Bin</t>
-  </si>
-  <si>
     <t>`</t>
   </si>
   <si>
@@ -64,23 +55,29 @@
     <t>F</t>
   </si>
   <si>
-    <t>Decimal -&gt;</t>
-  </si>
-  <si>
-    <t>Binary -&gt;</t>
-  </si>
-  <si>
-    <t>Octal -&gt;</t>
-  </si>
-  <si>
-    <t>Hexadecimal -&gt;</t>
+    <t>Your Hexadecimal Number:</t>
+  </si>
+  <si>
+    <t>Your Octal Number:</t>
+  </si>
+  <si>
+    <t>Your Binary Number:</t>
+  </si>
+  <si>
+    <t>Your Decimal Number:</t>
+  </si>
+  <si>
+    <t>Converted to Binary</t>
+  </si>
+  <si>
+    <t>The Amazing Number Convertor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,12 +117,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="JetBrains Mono NL Medium"/>
-      <family val="3"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
@@ -147,8 +138,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Amasis MT Pro Medium"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Amasis MT Pro Medium"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aharoni"/>
+      <charset val="177"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,8 +182,32 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -199,6 +239,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -208,15 +285,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="2" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyAlignment="1">
@@ -231,8 +305,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="2" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -245,6 +343,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF19105"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -553,16 +656,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A704EB-3FCB-4C58-B870-C2F844B63DB8}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
-    <col min="2" max="2" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
     <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" customWidth="1"/>
     <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
@@ -570,183 +673,190 @@
     <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="4"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="1">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="str">
-        <f>DEC2BIN(A2)</f>
-        <v>1010</v>
-      </c>
-      <c r="C2" s="1" t="str">
-        <f>DEC2OCT(A2)</f>
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="str">
-        <f>DEC2HEX(A2)</f>
-        <v>A</v>
-      </c>
+      <c r="D2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="7"/>
       <c r="F2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75">
-      <c r="D3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75">
-      <c r="A4" s="2" t="s">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="12">
+        <v>12</v>
+      </c>
+      <c r="B3" s="10" t="str">
+        <f>DEC2BIN(A3)</f>
+        <v>1100</v>
+      </c>
+      <c r="C3" s="11" t="str">
+        <f>DEC2OCT(A3)</f>
+        <v>14</v>
+      </c>
+      <c r="D3" s="9" t="str">
+        <f>DEC2HEX(A3)</f>
+        <v>C</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="D4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
+        <v>1010</v>
+      </c>
+      <c r="B6" s="11">
+        <f>BIN2DEC(A6)</f>
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C6" s="11" t="str">
+        <f>BIN2OCT(A6)</f>
+        <v>12</v>
+      </c>
+      <c r="D6" s="9" t="str">
+        <f>BIN2HEX(A6)</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C8" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="12">
+        <v>13</v>
+      </c>
+      <c r="B9" s="11">
+        <f>OCT2DEC(A9)</f>
+        <v>11</v>
+      </c>
+      <c r="C9" s="11" t="str">
+        <f>OCT2BIN(A9)</f>
+        <v>1011</v>
+      </c>
+      <c r="D9" s="9" t="str">
+        <f>OCT2HEX(A9)</f>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1">
-        <v>1010</v>
-      </c>
-      <c r="B5" s="1">
-        <f>BIN2DEC(A5)</f>
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="str">
-        <f>BIN2OCT(A5)</f>
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="str">
-        <f>BIN2HEX(A5)</f>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="C11" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D11" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="1">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1" t="str">
-        <f>OCT2BIN(A8)</f>
-        <v>1011</v>
-      </c>
-      <c r="C8" s="1">
-        <f>OCT2DEC(A8)</f>
-        <v>11</v>
-      </c>
-      <c r="D8" s="1" t="str">
-        <f>OCT2HEX(A8)</f>
-        <v>B</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="1" t="str">
-        <f>HEX2OCT(A11)</f>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="11" t="str">
+        <f>HEX2OCT(A12)</f>
         <v>17</v>
       </c>
-      <c r="C11" s="1" t="str">
-        <f>HEX2BIN(A11)</f>
+      <c r="C12" s="11" t="str">
+        <f>HEX2BIN(A12)</f>
         <v>1111</v>
       </c>
-      <c r="D11" s="1">
-        <f>HEX2DEC(A11)</f>
+      <c r="D12" s="9">
+        <f>HEX2DEC(A12)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="B13" s="6"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="B16" s="7"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="e">
-        <f>HEX2BIN(B23)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007479FE4EC35B1646BBA12FAF7AB7C336" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="41bd799682a802a6aba683020d2f45ed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fdec081d-d1af-4831-9470-36154f495fd7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="df8debe861c21b54100839cf6ef7f529" ns2:_="">
     <xsd:import namespace="fdec081d-d1af-4831-9470-36154f495fd7"/>
@@ -930,35 +1040,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7C0DA01-DCD9-420E-8E21-7DF7C551F369}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A72E30E9-6C09-4043-918F-BB66AD6737AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="fdec081d-d1af-4831-9470-36154f495fd7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -980,9 +1065,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A72E30E9-6C09-4043-918F-BB66AD6737AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7C0DA01-DCD9-420E-8E21-7DF7C551F369}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fdec081d-d1af-4831-9470-36154f495fd7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>